<commit_message>
Opening xlsx sheet function added
</commit_message>
<xml_diff>
--- a/Kostenoverzicht.xlsx
+++ b/Kostenoverzicht.xlsx
@@ -301,25 +301,25 @@
   <dimension ref="A1:R78"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.7397959183673"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.8010204081633"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -372,9 +372,7 @@
       <c r="R2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>2</v>
-      </c>
+      <c r="A3" s="4"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -574,7 +572,7 @@
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
-      <c r="P13" s="0"/>
+      <c r="P13" s="7"/>
       <c r="R13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>